<commit_message>
Simple Imag Obs + Simple Other Diag phase 2 added Diagnostic Report IG
Closes #45 and closes #48
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
   <si>
     <t>Path</t>
   </si>
@@ -419,52 +419,49 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
+  </si>
+  <si>
+    <t>FiveWs.what[x]</t>
+  </si>
+  <si>
+    <t>SPM-4/SPM-5</t>
+  </si>
+  <si>
+    <t>BodyStructure.location</t>
+  </si>
+  <si>
+    <t>Body site</t>
+  </si>
+  <si>
+    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
+  </si>
+  <si>
+    <t>.targetSiteCode</t>
+  </si>
+  <si>
+    <t>Name of location</t>
+  </si>
+  <si>
+    <t>OBX-20/SPM-8/SPM-10</t>
+  </si>
+  <si>
+    <t>BodyStructure.locationQualifier</t>
+  </si>
+  <si>
+    <t>Body site modifier</t>
+  </si>
+  <si>
+    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes describing anatomic morphology.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
-  </si>
-  <si>
-    <t>FiveWs.what[x]</t>
-  </si>
-  <si>
-    <t>SPM-4/SPM-5</t>
-  </si>
-  <si>
-    <t>BodyStructure.location</t>
-  </si>
-  <si>
-    <t>Body site</t>
-  </si>
-  <si>
-    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
-  </si>
-  <si>
-    <t>.targetSiteCode</t>
-  </si>
-  <si>
-    <t>Name of location</t>
-  </si>
-  <si>
-    <t>OBX-20/SPM-8/SPM-10</t>
-  </si>
-  <si>
-    <t>BodyStructure.locationQualifier</t>
-  </si>
-  <si>
-    <t>Body site modifier</t>
-  </si>
-  <si>
-    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2140,13 +2137,11 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" t="s" s="2">
         <v>128</v>
-      </c>
-      <c r="X13" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2185,15 +2180,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2219,10 +2214,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2249,11 +2244,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2271,7 +2266,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2286,21 +2281,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM14" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2326,10 +2321,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2356,14 +2351,14 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="X15" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="Y15" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="Y15" t="s" s="2">
-        <v>145</v>
-      </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2395,21 +2390,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM15" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2435,13 +2430,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2491,7 +2486,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2506,21 +2501,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>153</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2543,13 +2538,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2600,7 +2595,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2615,21 +2610,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2652,13 +2647,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>164</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2709,7 +2704,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2724,16 +2719,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="AK18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Base Practitioner in Diagnostic Report IG
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
   <si>
     <t>Path</t>
   </si>
@@ -419,6 +419,12 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes describing anatomic morphology.</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
   </si>
   <si>
@@ -459,9 +465,6 @@
   </si>
   <si>
     <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2137,11 +2140,13 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X13" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="X13" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="Y13" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2180,15 +2185,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2214,10 +2219,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2244,11 +2249,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2266,7 +2271,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2281,21 +2286,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2321,10 +2326,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2351,13 +2356,13 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
@@ -2375,7 +2380,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2390,21 +2395,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2430,13 +2435,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2486,7 +2491,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2501,21 +2506,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2538,13 +2543,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2595,7 +2600,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2610,21 +2615,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2647,13 +2652,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2704,7 +2709,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2719,16 +2724,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Atomic Pathology Observation profile
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
   <si>
     <t>Path</t>
   </si>
@@ -419,6 +419,12 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes describing anatomic morphology.</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
   </si>
   <si>
@@ -459,9 +465,6 @@
   </si>
   <si>
     <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2137,11 +2140,13 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X13" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="X13" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="Y13" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2180,15 +2185,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2214,10 +2219,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2244,11 +2249,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2266,7 +2271,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2281,21 +2286,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2321,10 +2326,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2351,13 +2356,13 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
@@ -2375,7 +2380,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2390,21 +2395,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2430,13 +2435,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2486,7 +2491,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2501,21 +2506,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2538,13 +2543,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2595,7 +2600,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2610,21 +2615,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2647,13 +2652,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2704,7 +2709,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2719,16 +2724,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Diagnostic Imaging Study in Diagnostic Report
Closes #52
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
   <si>
     <t>Path</t>
   </si>
@@ -419,52 +419,49 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
+  </si>
+  <si>
+    <t>FiveWs.what[x]</t>
+  </si>
+  <si>
+    <t>SPM-4/SPM-5</t>
+  </si>
+  <si>
+    <t>BodyStructure.location</t>
+  </si>
+  <si>
+    <t>Body site</t>
+  </si>
+  <si>
+    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
+  </si>
+  <si>
+    <t>.targetSiteCode</t>
+  </si>
+  <si>
+    <t>Name of location</t>
+  </si>
+  <si>
+    <t>OBX-20/SPM-8/SPM-10</t>
+  </si>
+  <si>
+    <t>BodyStructure.locationQualifier</t>
+  </si>
+  <si>
+    <t>Body site modifier</t>
+  </si>
+  <si>
+    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes describing anatomic morphology.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
-  </si>
-  <si>
-    <t>FiveWs.what[x]</t>
-  </si>
-  <si>
-    <t>SPM-4/SPM-5</t>
-  </si>
-  <si>
-    <t>BodyStructure.location</t>
-  </si>
-  <si>
-    <t>Body site</t>
-  </si>
-  <si>
-    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
-  </si>
-  <si>
-    <t>.targetSiteCode</t>
-  </si>
-  <si>
-    <t>Name of location</t>
-  </si>
-  <si>
-    <t>OBX-20/SPM-8/SPM-10</t>
-  </si>
-  <si>
-    <t>BodyStructure.locationQualifier</t>
-  </si>
-  <si>
-    <t>Body site modifier</t>
-  </si>
-  <si>
-    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2140,13 +2137,11 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" t="s" s="2">
         <v>128</v>
-      </c>
-      <c r="X13" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2185,15 +2180,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2219,10 +2214,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2249,11 +2244,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2271,7 +2266,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2286,21 +2281,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM14" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2326,10 +2321,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2356,14 +2351,14 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="X15" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="Y15" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="Y15" t="s" s="2">
-        <v>145</v>
-      </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2395,21 +2390,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM15" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2435,13 +2430,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2491,7 +2486,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2506,21 +2501,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>153</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2543,13 +2538,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2600,7 +2595,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2615,21 +2610,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2652,13 +2647,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>164</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2709,7 +2704,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2724,16 +2719,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="AK18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Base BodyStructure in Diagnostic Report IG
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -157,7 +157,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-bodstr-0:The body structure shall at least have a location or a description or an image {location.exists() or description.exists() or image.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-bodstr-0:The body structure shall at least have a location or a description or an image {location.exists() or description.exists() or image.exists()}inv-dh-bodstr-01:The patient shall at least have a reference or an identifier with at least a system and a value {patient.reference.exists() or patient.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-bodstr-02:The body structure shall at least have a location or a description {location.exists() or description.exists()}</t>
   </si>
   <si>
     <t>ActSIte</t>
@@ -437,7 +437,7 @@
     <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
   </si>
   <si>
-    <t>extensible</t>
+    <t>required</t>
   </si>
   <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
@@ -522,7 +522,7 @@
     <t>BodyStructure.patient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Diagnostic Report IG - first draft of R4 Base PractitionerRole Diagnostic Report IG and Event Summary IG - PractitionerRole with Mandatory Identifier :: phase 2
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
   <si>
     <t>Path</t>
   </si>
@@ -419,6 +419,12 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes describing anatomic morphology.</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
   </si>
   <si>
@@ -459,9 +465,6 @@
   </si>
   <si>
     <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2137,11 +2140,13 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X13" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="X13" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="Y13" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2180,15 +2185,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2214,10 +2219,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2244,11 +2249,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2266,7 +2271,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2281,21 +2286,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2321,10 +2326,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2351,13 +2356,13 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
@@ -2375,7 +2380,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2390,21 +2395,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2430,13 +2435,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2486,7 +2491,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2501,21 +2506,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2538,13 +2543,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2595,7 +2600,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2610,21 +2615,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2647,13 +2652,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2704,7 +2709,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2719,16 +2724,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drafted FBC + ESR examples (Atomic + MHR) + atomic imag obs phase 2
Closes #51 and Closes #77 and Closes#76
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
+++ b/output/DiagnosticReport/bodystructure-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="168">
   <si>
     <t>Path</t>
   </si>
@@ -419,52 +419,49 @@
     <t>The minimum cardinality of 0 supports the use case of specifying a location without defining a morphology.</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
+  </si>
+  <si>
+    <t>FiveWs.what[x]</t>
+  </si>
+  <si>
+    <t>SPM-4/SPM-5</t>
+  </si>
+  <si>
+    <t>BodyStructure.location</t>
+  </si>
+  <si>
+    <t>Body site</t>
+  </si>
+  <si>
+    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
+  </si>
+  <si>
+    <t>.targetSiteCode</t>
+  </si>
+  <si>
+    <t>Name of location</t>
+  </si>
+  <si>
+    <t>OBX-20/SPM-8/SPM-10</t>
+  </si>
+  <si>
+    <t>BodyStructure.locationQualifier</t>
+  </si>
+  <si>
+    <t>Body site modifier</t>
+  </si>
+  <si>
+    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes describing anatomic morphology.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/bodystructure-code</t>
-  </si>
-  <si>
-    <t>FiveWs.what[x]</t>
-  </si>
-  <si>
-    <t>SPM-4/SPM-5</t>
-  </si>
-  <si>
-    <t>BodyStructure.location</t>
-  </si>
-  <si>
-    <t>Body site</t>
-  </si>
-  <si>
-    <t>The anatomical location or region of the specimen, lesion, or body structure.</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
-  </si>
-  <si>
-    <t>.targetSiteCode</t>
-  </si>
-  <si>
-    <t>Name of location</t>
-  </si>
-  <si>
-    <t>OBX-20/SPM-8/SPM-10</t>
-  </si>
-  <si>
-    <t>BodyStructure.locationQualifier</t>
-  </si>
-  <si>
-    <t>Body site modifier</t>
-  </si>
-  <si>
-    <t>Qualifier to refine the anatomical location.  These include qualifiers for laterality, relative location, directionality, number, and plane.</t>
   </si>
   <si>
     <t>Concepts modifying the anatomic location.</t>
@@ -2140,13 +2137,11 @@
         <v>43</v>
       </c>
       <c r="W13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" t="s" s="2">
         <v>128</v>
-      </c>
-      <c r="X13" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
@@ -2185,15 +2180,15 @@
         <v>43</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2219,10 +2214,10 @@
         <v>124</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2249,11 +2244,11 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -2271,7 +2266,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2286,21 +2281,21 @@
         <v>62</v>
       </c>
       <c r="AJ14" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM14" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2326,10 +2321,10 @@
         <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2356,14 +2351,14 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="X15" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="Y15" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="Y15" t="s" s="2">
-        <v>145</v>
-      </c>
       <c r="Z15" t="s" s="2">
         <v>43</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2395,21 +2390,21 @@
         <v>62</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM15" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2435,13 +2430,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2491,7 +2486,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2506,21 +2501,21 @@
         <v>62</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>153</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2543,13 +2538,13 @@
         <v>43</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2600,7 +2595,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2615,21 +2610,21 @@
         <v>62</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2652,13 +2647,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>164</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2709,7 +2704,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>50</v>
@@ -2724,16 +2719,16 @@
         <v>62</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="AK18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>